<commit_message>
written moscow requirement, and hardware
</commit_message>
<xml_diff>
--- a/Gantt Chart v3.xlsx
+++ b/Gantt Chart v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mhby1g21_soton_ac_uk/Documents/COURSES/Y3/COMP3200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{FDC4CFA3-C157-4A7B-8E8E-45EC873C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9D5F163-2114-4FE7-B293-44C0D39D7266}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{FDC4CFA3-C157-4A7B-8E8E-45EC873C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F04937BF-469C-43A3-ACEC-271AF119F894}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important dates" sheetId="4" r:id="rId1"/>
@@ -4436,16 +4436,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:rowOff>42861</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5845,7 +5845,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,7 +6362,7 @@
         <v>45257</v>
       </c>
       <c r="E22" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added kicad library, papers and progressreport overleaf pdf
</commit_message>
<xml_diff>
--- a/Gantt Chart v3.xlsx
+++ b/Gantt Chart v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mhby1g21_soton_ac_uk/Documents/COURSES/Y3/COMP3200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{FDC4CFA3-C157-4A7B-8E8E-45EC873C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F04937BF-469C-43A3-ACEC-271AF119F894}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{FDC4CFA3-C157-4A7B-8E8E-45EC873C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5081F82B-C7C2-4667-87E0-77E61322B47C}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4784,7 +4784,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4858,7 +4858,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>45271</v>
+        <v>45275</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -4867,7 +4867,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F4" t="s">
         <v>87</v>
@@ -4887,7 +4887,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
@@ -5845,7 +5845,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6317,7 +6317,7 @@
         <v>45246</v>
       </c>
       <c r="E20" s="2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F20" t="s">
         <v>103</v>
@@ -6355,14 +6355,14 @@
         <v>45254</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>45257</v>
+        <v>45267</v>
       </c>
       <c r="E22" s="2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added lots to progress report
</commit_message>
<xml_diff>
--- a/Gantt Chart v3.xlsx
+++ b/Gantt Chart v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mhby1g21_soton_ac_uk/Documents/COURSES/Y3/COMP3200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{FDC4CFA3-C157-4A7B-8E8E-45EC873C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5081F82B-C7C2-4667-87E0-77E61322B47C}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{FDC4CFA3-C157-4A7B-8E8E-45EC873C3CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA8040CA-6775-4098-BE15-E9804E1778A0}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="1755" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important dates" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="105">
   <si>
     <t>Project Management Gantt Chart</t>
   </si>
@@ -209,12 +209,6 @@
     <t>submit request and wait till get component</t>
   </si>
   <si>
-    <t>Draft Project Report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start drafting on latex </t>
-  </si>
-  <si>
     <t>Software prototype documentation (SPDOC1)</t>
   </si>
   <si>
@@ -357,6 +351,9 @@
   </si>
   <si>
     <t>Progress Report Writeup</t>
+  </si>
+  <si>
+    <t>ELEC Coursework</t>
   </si>
 </sst>
 </file>
@@ -471,9 +468,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Planned!$A$4:$A$54</c:f>
+              <c:f>Planned!$A$4:$A$53</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
@@ -499,72 +496,69 @@
                   <c:v>Design document drafting p1 (DD1)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Draft Project Report</c:v>
+                  <c:v>Hardware procurement  </c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Hardware procurement  </c:v>
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                  <c:v>SPDEV2: Stereo image and video</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>SPDEV2: Stereo image and video</c:v>
+                  <c:v>SPT2: Stereo 3DS video and image test</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>SPT2: Stereo 3DS video and image test</c:v>
+                  <c:v>Embedded Hardware Programming study</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Embedded Hardware Programming study</c:v>
+                  <c:v>Hardware prototype development (HPDEV1): Basic Mono Functions</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Hardware prototype development (HPDEV1): Basic Mono Functions</c:v>
+                  <c:v>Hardware prototype testing (HPT1): Mono Testing</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Hardware prototype testing (HPT1): Mono Testing</c:v>
+                  <c:v>HPDOC2: Reflections and problems faced</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>HPDOC2: Reflections and problems faced</c:v>
+                  <c:v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</c:v>
+                  <c:v>SPT3: Pico Camera images and video test (resolution changes)</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>SPT3: Pico Camera images and video test (resolution changes)</c:v>
+                  <c:v>HPR2: 3D Modelling Software Study and training</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>HPR2: 3D Modelling Software Study and training</c:v>
+                  <c:v>HPDEV2: 3D model design v1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>HPDEV2: 3D model design v1</c:v>
+                  <c:v>EXAM WEEKS</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>EXAM WEEKS</c:v>
+                  <c:v>HPDEV3: Stereo camera functionality</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>HPDEV3: Stereo camera functionality</c:v>
+                  <c:v>HPT3: Functional hardware test to get footage</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>HPT3: Functional hardware test to get footage</c:v>
+                  <c:v>SPDEV3: Stereo audio sync and optimisation</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>SPDEV3: Stereo audio sync and optimisation</c:v>
+                  <c:v>SPT3: Testing on friends for feedback</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>SPT3: Testing on friends for feedback</c:v>
+                  <c:v>HPDEV4: Add onboard battery (and charging circuit)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>HPDEV4: Add onboard battery (and charging circuit)</c:v>
+                  <c:v>HPT4: Test onboard battery life and powermode </c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>HPT4: Test onboard battery life and powermode </c:v>
+                  <c:v>Optimisation and organisation</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Optimisation and organisation</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Final report write up</c:v>
                 </c:pt>
               </c:strCache>
@@ -572,10 +566,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planned!$B$4:$B$34</c:f>
+              <c:f>Planned!$B$4:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>45201</c:v>
                 </c:pt>
@@ -601,72 +595,69 @@
                   <c:v>45211</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45212</c:v>
+                  <c:v>45215</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45215</c:v>
+                  <c:v>45216</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45216</c:v>
+                  <c:v>45223</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45223</c:v>
+                  <c:v>45218</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45218</c:v>
+                  <c:v>45232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45232</c:v>
+                  <c:v>45235</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45235</c:v>
+                  <c:v>45242</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>45242</c:v>
+                  <c:v>45256</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45256</c:v>
+                  <c:v>45259</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45259</c:v>
+                  <c:v>45261</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>45261</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>45275</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="d\-mmm">
+                <c:pt idx="19" formatCode="d\-mmm">
                   <c:v>45280</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>45294</c:v>
+                </c:pt>
                 <c:pt idx="21">
-                  <c:v>45294</c:v>
+                  <c:v>45299</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45299</c:v>
+                  <c:v>45320</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>45320</c:v>
+                  <c:v>45327</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>45327</c:v>
+                  <c:v>45334</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>45334</c:v>
+                  <c:v>45341</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>45341</c:v>
+                  <c:v>45344</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>45344</c:v>
+                  <c:v>45354</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>45354</c:v>
+                  <c:v>45361</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>45361</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>45366</c:v>
                 </c:pt>
               </c:numCache>
@@ -798,12 +789,26 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="9"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -879,7 +884,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -931,23 +936,18 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="16"/>
+            <c:idx val="17"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-1B7F-4994-A620-2F67083514CA}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -974,7 +974,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1012,7 +1012,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1031,7 +1031,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1069,7 +1069,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1107,7 +1107,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1139,30 +1139,11 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="28"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000017-1B7F-4994-A620-2F67083514CA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Planned!$A$4:$A$54</c:f>
+              <c:f>Planned!$A$4:$A$53</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
@@ -1188,72 +1169,69 @@
                   <c:v>Design document drafting p1 (DD1)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Draft Project Report</c:v>
+                  <c:v>Hardware procurement  </c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Hardware procurement  </c:v>
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                  <c:v>SPDEV2: Stereo image and video</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>SPDEV2: Stereo image and video</c:v>
+                  <c:v>SPT2: Stereo 3DS video and image test</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>SPT2: Stereo 3DS video and image test</c:v>
+                  <c:v>Embedded Hardware Programming study</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Embedded Hardware Programming study</c:v>
+                  <c:v>Hardware prototype development (HPDEV1): Basic Mono Functions</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Hardware prototype development (HPDEV1): Basic Mono Functions</c:v>
+                  <c:v>Hardware prototype testing (HPT1): Mono Testing</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Hardware prototype testing (HPT1): Mono Testing</c:v>
+                  <c:v>HPDOC2: Reflections and problems faced</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>HPDOC2: Reflections and problems faced</c:v>
+                  <c:v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</c:v>
+                  <c:v>SPT3: Pico Camera images and video test (resolution changes)</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>SPT3: Pico Camera images and video test (resolution changes)</c:v>
+                  <c:v>HPR2: 3D Modelling Software Study and training</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>HPR2: 3D Modelling Software Study and training</c:v>
+                  <c:v>HPDEV2: 3D model design v1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>HPDEV2: 3D model design v1</c:v>
+                  <c:v>EXAM WEEKS</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>EXAM WEEKS</c:v>
+                  <c:v>HPDEV3: Stereo camera functionality</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>HPDEV3: Stereo camera functionality</c:v>
+                  <c:v>HPT3: Functional hardware test to get footage</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>HPT3: Functional hardware test to get footage</c:v>
+                  <c:v>SPDEV3: Stereo audio sync and optimisation</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>SPDEV3: Stereo audio sync and optimisation</c:v>
+                  <c:v>SPT3: Testing on friends for feedback</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>SPT3: Testing on friends for feedback</c:v>
+                  <c:v>HPDEV4: Add onboard battery (and charging circuit)</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>HPDEV4: Add onboard battery (and charging circuit)</c:v>
+                  <c:v>HPT4: Test onboard battery life and powermode </c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>HPT4: Test onboard battery life and powermode </c:v>
+                  <c:v>Optimisation and organisation</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Optimisation and organisation</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Final report write up</c:v>
                 </c:pt>
               </c:strCache>
@@ -1261,10 +1239,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planned!$C$4:$C$34</c:f>
+              <c:f>Planned!$C$4:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1290,72 +1268,69 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="28">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
@@ -2057,7 +2032,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planned!$B$3</c:f>
+              <c:f>Combined!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2076,9 +2051,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Executed!$A$4:$A$11</c:f>
+              <c:f>Combined!$A$4:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
@@ -2102,16 +2077,46 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hardware procurement  </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Learning LaTeX</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SPDEV2: Stereo image and video</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SPT2: Stereo footage video and image test</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Embedded Hardware Programming study</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Hardware component testing</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ELEC Coursework</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Progress Report Writeup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planned!$B$4:$B$11</c:f>
+              <c:f>Combined!$B$4:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>45201</c:v>
                 </c:pt>
@@ -2131,10 +2136,40 @@
                   <c:v>45207</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45209</c:v>
+                  <c:v>45210</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45211</c:v>
+                  <c:v>45214</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45215</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45217</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45223</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45218</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45232</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45235</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45238</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45246</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2264,11 +2299,106 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001C-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001E-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Executed!$A$4:$A$11</c:f>
+              <c:f>Combined!$A$4:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
@@ -2292,16 +2422,46 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hardware procurement  </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Learning LaTeX</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SPDEV2: Stereo image and video</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SPT2: Stereo footage video and image test</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Embedded Hardware Programming study</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Hardware component testing</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ELEC Coursework</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Progress Report Writeup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Combined!$C$4:$C$11</c:f>
+              <c:f>Combined!$C$4:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2325,6 +2485,36 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2513,11 +2703,164 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001A-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000020-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000022-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-10EE-4C46-B2BD-4923B7CF5534}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Executed!$A$4:$A$11</c:f>
+              <c:f>Combined!$A$4:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Literature research</c:v>
                 </c:pt>
@@ -2541,16 +2884,46 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Design document drafting p1 (DD1)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Hardware procurement  </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Learning LaTeX</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SPR2: Stereo and OpenXR implementation</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Software prototype documentation (SPDOC1)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SPDEV2: Stereo image and video</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SPT2: Stereo footage video and image test</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Embedded Hardware Programming study</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Hardware component testing</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ELEC Coursework</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Progress Report Writeup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Combined!$E$4:$E$11</c:f>
+              <c:f>Combined!$E$4:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -2574,6 +2947,36 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4397,13 +4800,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4444,7 +4847,7 @@
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4480,15 +4883,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>97877</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>84739</xdr:rowOff>
+      <xdr:colOff>364576</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>316953</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>32350</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4850,7 +5253,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4870,7 +5273,7 @@
         <v>0.1</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4907,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -5047,10 +5450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5141,7 +5544,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D43" si="0">B5+C5</f>
+        <f t="shared" ref="D5:D42" si="0">B5+C5</f>
         <v>45204</v>
       </c>
       <c r="E5" s="2">
@@ -5283,7 +5686,7 @@
         <v>Yes</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5314,17 +5717,17 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1">
-        <v>45212</v>
+        <v>45215</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>45214</v>
+        <v>45229</v>
       </c>
       <c r="E12" s="2">
         <f>Executed!E12</f>
@@ -5335,22 +5738,22 @@
         <v>Yes</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1">
-        <v>45215</v>
+        <v>45216</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>45229</v>
+        <v>45223</v>
       </c>
       <c r="E13" s="2">
         <f>Executed!E13</f>
@@ -5360,23 +5763,20 @@
         <f>Executed!F13</f>
         <v>Yes</v>
       </c>
-      <c r="G13" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1">
-        <v>45216</v>
+        <v>45223</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="E14" s="2">
         <f>Executed!E14</f>
@@ -5387,65 +5787,65 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1">
-        <v>45223</v>
+        <v>45218</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>45230</v>
+        <v>45232</v>
       </c>
       <c r="E15" s="2">
         <f>Executed!E15</f>
-        <v>1</v>
-      </c>
-      <c r="F15" t="str">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <f>Executed!F15</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1">
-        <v>45218</v>
+        <v>45232</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>45232</v>
+        <v>45235</v>
       </c>
       <c r="E16" s="2">
         <f>Executed!E16</f>
-        <v>0</v>
-      </c>
-      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="str">
         <f>Executed!F16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1">
-        <v>45232</v>
+        <v>45235</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>45235</v>
+        <v>45242</v>
       </c>
       <c r="E17" s="2">
         <f>Executed!E17</f>
@@ -5455,20 +5855,23 @@
         <f>Executed!F17</f>
         <v>Yes</v>
       </c>
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1">
-        <v>45235</v>
+        <v>45242</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>45242</v>
+        <v>45256</v>
       </c>
       <c r="E18" s="2">
         <f>Executed!E18</f>
@@ -5479,33 +5882,33 @@
         <v>Yes</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1">
-        <v>45242</v>
+        <v>45256</v>
       </c>
       <c r="C19">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>45256</v>
+        <v>45259</v>
       </c>
       <c r="E19" s="2">
-        <f>Executed!E19</f>
-        <v>1</v>
-      </c>
-      <c r="F19" t="str">
-        <f>Executed!F19</f>
-        <v>Yes</v>
+        <f>Executed!E22</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>Executed!F22</f>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5513,14 +5916,14 @@
         <v>65</v>
       </c>
       <c r="B20" s="1">
-        <v>45256</v>
+        <v>45259</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>45259</v>
+        <v>45261</v>
       </c>
       <c r="E20" s="2">
         <f>Executed!E23</f>
@@ -5530,46 +5933,39 @@
         <f>Executed!F23</f>
         <v>0</v>
       </c>
-      <c r="G20" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1">
-        <v>45259</v>
+        <v>45261</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>45261</v>
+        <v>45275</v>
       </c>
       <c r="E21" s="2">
         <f>Executed!E24</f>
         <v>0</v>
       </c>
-      <c r="F21">
-        <f>Executed!F24</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="1">
-        <v>45261</v>
+        <v>45275</v>
       </c>
       <c r="C22">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>45275</v>
+        <v>45278</v>
       </c>
       <c r="E22" s="2">
         <f>Executed!E25</f>
@@ -5578,17 +5974,17 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="1">
-        <v>45275</v>
+        <v>69</v>
+      </c>
+      <c r="B23" s="5">
+        <v>45280</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>45278</v>
+        <v>45294</v>
       </c>
       <c r="E23" s="2">
         <f>Executed!E26</f>
@@ -5599,15 +5995,15 @@
       <c r="A24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="5">
-        <v>45280</v>
+      <c r="B24" s="1">
+        <v>45294</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>45294</v>
+        <v>45299</v>
       </c>
       <c r="E24" s="2">
         <f>Executed!E27</f>
@@ -5616,21 +6012,20 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45299</v>
+      </c>
+      <c r="C25">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>45320</v>
+      </c>
+      <c r="G25" t="s">
         <v>73</v>
-      </c>
-      <c r="B25" s="1">
-        <v>45294</v>
-      </c>
-      <c r="C25">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="0"/>
-        <v>45299</v>
-      </c>
-      <c r="E25" s="2">
-        <f>Executed!E28</f>
-        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5638,17 +6033,17 @@
         <v>72</v>
       </c>
       <c r="B26" s="1">
-        <v>45299</v>
+        <v>45320</v>
       </c>
       <c r="C26">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>45320</v>
+        <v>45334</v>
       </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5656,125 +6051,113 @@
         <v>74</v>
       </c>
       <c r="B27" s="1">
-        <v>45320</v>
+        <v>45327</v>
       </c>
       <c r="C27">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
         <v>45334</v>
       </c>
       <c r="G27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B28" s="1">
-        <v>45327</v>
+        <v>45334</v>
       </c>
       <c r="C28">
         <v>7</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>45334</v>
-      </c>
-      <c r="G28" t="s">
-        <v>77</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1">
-        <v>45334</v>
+        <v>45341</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>45341</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1">
-        <v>45341</v>
+        <v>45344</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>45344</v>
+        <v>45354</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="1">
-        <v>45344</v>
+        <v>45354</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>45354</v>
+        <v>45361</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1">
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="C32">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>45361</v>
+        <v>45366</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="1">
-        <v>45361</v>
+        <v>45366</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>45366</v>
+        <v>45387</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="1">
-        <v>45366</v>
-      </c>
-      <c r="C34">
-        <v>21</v>
-      </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>45387</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5821,12 +6204,6 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5842,10 +6219,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F12609-C238-4402-9A8B-B1D994A238B7}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,7 +6299,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5938,7 +6315,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D38" si="0">B5+C5</f>
+        <f t="shared" ref="D5:D37" si="0">B5+C5</f>
         <v>45207</v>
       </c>
       <c r="E5" s="2">
@@ -6055,7 +6432,7 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -6083,7 +6460,7 @@
         <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6108,23 +6485,24 @@
         <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Planned!A12</f>
-        <v>Draft Project Report</v>
+        <v xml:space="preserve">Hardware procurement  </v>
       </c>
       <c r="B12" s="1">
+        <f>Planned!B12</f>
         <v>45215</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>45216</v>
+        <v>45222</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -6132,22 +6510,23 @@
       <c r="F12" t="s">
         <v>17</v>
       </c>
+      <c r="G12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>Planned!A13</f>
-        <v xml:space="preserve">Hardware procurement  </v>
+      <c r="A13" t="s">
+        <v>89</v>
       </c>
       <c r="B13" s="1">
-        <f>Planned!B13</f>
-        <v>45215</v>
+        <v>45217</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>45222</v>
+        <v>45231</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -6156,22 +6535,24 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>91</v>
+      <c r="A14" t="str">
+        <f>Planned!A13</f>
+        <v>SPR2: Stereo and OpenXR implementation</v>
       </c>
       <c r="B14" s="1">
-        <v>45217</v>
+        <f>Planned!B13</f>
+        <v>45216</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>45231</v>
+        <v>45234</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -6180,67 +6561,65 @@
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>Planned!A14</f>
-        <v>SPR2: Stereo and OpenXR implementation</v>
+        <v>Software prototype documentation (SPDOC1)</v>
       </c>
       <c r="B15" s="1">
         <f>Planned!B14</f>
-        <v>45216</v>
-      </c>
-      <c r="C15">
-        <v>18</v>
+        <v>45223</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>45234</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" t="s">
-        <v>97</v>
+        <v>45223</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>Planned!A15</f>
-        <v>Software prototype documentation (SPDOC1)</v>
+        <v>SPDEV2: Stereo image and video</v>
       </c>
       <c r="B16" s="1">
         <f>Planned!B15</f>
-        <v>45223</v>
+        <v>45218</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>45223</v>
+        <v>45234</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>Planned!A16</f>
-        <v>SPDEV2: Stereo image and video</v>
+      <c r="A17" t="s">
+        <v>97</v>
       </c>
       <c r="B17" s="1">
-        <f>Planned!B16</f>
-        <v>45218</v>
+        <v>45232</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>45234</v>
+        <v>45235</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
@@ -6249,22 +6628,24 @@
         <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
+      <c r="A18" t="str">
+        <f>Planned!A17</f>
+        <v>Embedded Hardware Programming study</v>
       </c>
       <c r="B18" s="1">
-        <v>45232</v>
+        <f>Planned!B17</f>
+        <v>45235</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>45235</v>
+        <v>45245</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
@@ -6277,29 +6658,27 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f>Planned!A18</f>
-        <v>Embedded Hardware Programming study</v>
+      <c r="A19" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="1">
-        <f>Planned!B18</f>
-        <v>45235</v>
+        <v>45238</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>45245</v>
+        <v>45246</v>
       </c>
       <c r="E19" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="G19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6307,287 +6686,263 @@
         <v>102</v>
       </c>
       <c r="B20" s="1">
-        <v>45238</v>
+        <v>45246</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>45246</v>
+        <v>45252</v>
       </c>
       <c r="E20" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
-      </c>
-      <c r="G20" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="1">
-        <v>45246</v>
+        <v>45254</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>45252</v>
+        <v>45267</v>
       </c>
       <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>105</v>
+      <c r="A22" t="str">
+        <f>Planned!A18</f>
+        <v>Hardware prototype development (HPDEV1): Basic Mono Functions</v>
       </c>
       <c r="B22" s="1">
-        <v>45254</v>
+        <f>Planned!B18</f>
+        <v>45242</v>
       </c>
       <c r="C22">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>45267</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.5</v>
+        <v>45242</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>Planned!A19</f>
-        <v>Hardware prototype development (HPDEV1): Basic Mono Functions</v>
+        <v>Hardware prototype testing (HPT1): Mono Testing</v>
       </c>
       <c r="B23" s="1">
         <f>Planned!B19</f>
-        <v>45242</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+        <v>45256</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>45242</v>
+        <v>45256</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>Planned!A20</f>
-        <v>Hardware prototype testing (HPT1): Mono Testing</v>
+        <v>HPDOC2: Reflections and problems faced</v>
       </c>
       <c r="B24" s="1">
         <f>Planned!B20</f>
-        <v>45256</v>
+        <v>45259</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>45256</v>
+        <v>45259</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>Planned!A21</f>
-        <v>HPDOC2: Reflections and problems faced</v>
+        <v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</v>
       </c>
       <c r="B25" s="1">
         <f>Planned!B21</f>
-        <v>45259</v>
+        <v>45261</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>45259</v>
+        <v>45261</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>Planned!A22</f>
-        <v>SPDEV3: Image timelapse browsing (mono) and video playback (UI)</v>
+        <v>SPT3: Pico Camera images and video test (resolution changes)</v>
       </c>
       <c r="B26" s="1">
         <f>Planned!B22</f>
-        <v>45261</v>
+        <v>45275</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>45261</v>
+        <v>45275</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>Planned!A23</f>
-        <v>SPT3: Pico Camera images and video test (resolution changes)</v>
+        <v>HPR2: 3D Modelling Software Study and training</v>
       </c>
       <c r="B27" s="1">
         <f>Planned!B23</f>
-        <v>45275</v>
+        <v>45280</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>45275</v>
+        <v>45280</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>Planned!A24</f>
-        <v>HPR2: 3D Modelling Software Study and training</v>
+        <v>HPDEV2: 3D model design v1</v>
       </c>
       <c r="B28" s="1">
         <f>Planned!B24</f>
-        <v>45280</v>
+        <v>45294</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>45280</v>
+        <v>45294</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>Planned!A25</f>
-        <v>HPDEV2: 3D model design v1</v>
+        <v>EXAM WEEKS</v>
       </c>
       <c r="B29" s="1">
         <f>Planned!B25</f>
-        <v>45294</v>
+        <v>45299</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>45294</v>
+        <v>45299</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>Planned!A26</f>
-        <v>EXAM WEEKS</v>
+        <v>HPDEV3: Stereo camera functionality</v>
       </c>
       <c r="B30" s="1">
         <f>Planned!B26</f>
-        <v>45299</v>
+        <v>45320</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>45299</v>
+        <v>45320</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>Planned!A27</f>
-        <v>HPDEV3: Stereo camera functionality</v>
+        <v>HPT3: Functional hardware test to get footage</v>
       </c>
       <c r="B31" s="1">
         <f>Planned!B27</f>
-        <v>45320</v>
+        <v>45327</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>45320</v>
+        <v>45327</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>Planned!A28</f>
-        <v>HPT3: Functional hardware test to get footage</v>
+        <v>SPDEV3: Stereo audio sync and optimisation</v>
       </c>
       <c r="B32" s="1">
         <f>Planned!B28</f>
-        <v>45327</v>
+        <v>45334</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>45327</v>
+        <v>45334</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>Planned!A29</f>
-        <v>SPDEV3: Stereo audio sync and optimisation</v>
+        <v>SPT3: Testing on friends for feedback</v>
       </c>
       <c r="B33" s="1">
         <f>Planned!B29</f>
-        <v>45334</v>
+        <v>45341</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>45334</v>
+        <v>45341</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>Planned!A30</f>
-        <v>SPT3: Testing on friends for feedback</v>
+        <v>HPDEV4: Add onboard battery (and charging circuit)</v>
       </c>
       <c r="B34" s="1">
         <f>Planned!B30</f>
-        <v>45341</v>
+        <v>45344</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>45341</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>Planned!A31</f>
-        <v>HPDEV4: Add onboard battery (and charging circuit)</v>
+        <v xml:space="preserve">HPT4: Test onboard battery life and powermode </v>
       </c>
       <c r="B35" s="1">
         <f>Planned!B31</f>
-        <v>45344</v>
+        <v>45354</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="0"/>
-        <v>45344</v>
+        <v>45354</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>Planned!A32</f>
-        <v xml:space="preserve">HPT4: Test onboard battery life and powermode </v>
+        <v>Optimisation and organisation</v>
       </c>
       <c r="B36" s="1">
         <f>Planned!B32</f>
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="0"/>
-        <v>45354</v>
+        <v>45361</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>Planned!A33</f>
-        <v>Optimisation and organisation</v>
+        <v>Final report write up</v>
       </c>
       <c r="B37" s="1">
         <f>Planned!B33</f>
-        <v>45361</v>
+        <v>45366</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="0"/>
-        <v>45361</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="str">
-        <f>Planned!A34</f>
-        <v>Final report write up</v>
-      </c>
-      <c r="B38" s="1">
-        <f>Planned!B34</f>
-        <v>45366</v>
-      </c>
-      <c r="D38" s="1">
         <f t="shared" si="0"/>
         <v>45366</v>
       </c>
@@ -6605,15 +6960,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB32B44-AF31-4750-897C-7301F24D334D}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="4" customWidth="1"/>
@@ -6697,7 +7053,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E11" si="0">IF(D5-C5&lt;0, 0, D5-C5)</f>
+        <f t="shared" ref="E5:E21" si="0">IF(D5-C5&lt;0, 0, D5-C5)</f>
         <v>3</v>
       </c>
     </row>
@@ -6813,24 +7169,232 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>Executed!A11</f>
+        <f>Planned!A11</f>
         <v>Design document drafting p1 (DD1)</v>
       </c>
       <c r="B11" s="1">
-        <f>Executed!B11</f>
         <v>45214</v>
       </c>
       <c r="C11">
-        <f>Planned!C11</f>
         <v>3</v>
       </c>
       <c r="D11">
-        <f>Executed!C11</f>
         <v>1</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>Planned!A12</f>
+        <v xml:space="preserve">Hardware procurement  </v>
+      </c>
+      <c r="B12" s="1">
+        <f>Planned!B12</f>
+        <v>45215</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4">
+        <f>IF(D12-C12&lt;0, 0, D12-C12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45217</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4">
+        <f>IF(D13-C13&lt;0, 0, D13-C13)</f>
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>Planned!A13</f>
+        <v>SPR2: Stereo and OpenXR implementation</v>
+      </c>
+      <c r="B14" s="1">
+        <f>Planned!B13</f>
+        <v>45216</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>Planned!A14</f>
+        <v>Software prototype documentation (SPDOC1)</v>
+      </c>
+      <c r="B15" s="1">
+        <f>Planned!B14</f>
+        <v>45223</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>Planned!A15</f>
+        <v>SPDEV2: Stereo image and video</v>
+      </c>
+      <c r="B16" s="1">
+        <f>Planned!B15</f>
+        <v>45218</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45232</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>Planned!A17</f>
+        <v>Embedded Hardware Programming study</v>
+      </c>
+      <c r="B18" s="1">
+        <f>Planned!B17</f>
+        <v>45235</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45238</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45246</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45254</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>